<commit_message>
Added _generated tag to generated Openscenario files
They are now gitignored based on this new tag.
Also fixed an issue with the copy of the folder in OpenScnario API_main
</commit_message>
<xml_diff>
--- a/AD-EYE/TA/Configurations/TAOrder.xlsx
+++ b/AD-EYE/TA/Configurations/TAOrder.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adeye\AD-EYE_Core\AD-EYE\TA\Configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{438E42D1-3D3C-4DE6-93F1-ABA41B102D49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{739E4993-3EE9-4703-8C5F-38D4A6821D16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15996" yWindow="1272" windowWidth="14724" windowHeight="12204" xr2:uid="{6A716585-B476-48DA-845D-AAEABE8F85A6}"/>
   </bookViews>
@@ -104,10 +104,10 @@
     <t>AutowareConfigTemplate_6.xlsx</t>
   </si>
   <si>
-    <t>KTH_pedestrian_autoware_light/OpenScenario/Results/Experiment_A1/OpenScenario</t>
-  </si>
-  <si>
-    <t>KTH_pedestrian_autoware_light/OpenScenario/Results/Experiment_A2/OpenScenario</t>
+    <t>KTH_pedestrian_autoware_light/OpenScenario/Results/Experiment_A1_generated/OpenScenario</t>
+  </si>
+  <si>
+    <t>KTH_pedestrian_autoware_light/OpenScenario/Results/Experiment_A2_generated/OpenScenario</t>
   </si>
 </sst>
 </file>
@@ -466,7 +466,7 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="49" width="72.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="49" width="82.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:49" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Removed duplication of goal in TA
</commit_message>
<xml_diff>
--- a/AD-EYE/TA/Configurations/TAOrder.xlsx
+++ b/AD-EYE/TA/Configurations/TAOrder.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adeye\AD-EYE_Core\AD-EYE\TA\Configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5B9A3CFC-8F24-4F8D-BCF3-4DC6BE8AE758}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{32C8E28C-5255-452D-B366-2D7C1C855E66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15996" yWindow="1272" windowWidth="14724" windowHeight="12204" xr2:uid="{6A716585-B476-48DA-845D-AAEABE8F85A6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="22">
   <si>
     <t>FolderExpName</t>
   </si>
@@ -50,9 +50,6 @@
     <t>AutowareConfig</t>
   </si>
   <si>
-    <t>GoalConfig</t>
-  </si>
-  <si>
     <t>SimulinkConfig</t>
   </si>
   <si>
@@ -62,6 +59,9 @@
     <t>SHHConfig</t>
   </si>
   <si>
+    <t>KTH_pedestrian_autoware_light/OpenScenario/Results/Experiment_A1_generated/OpenScenario</t>
+  </si>
+  <si>
     <t>KTH_pedestrian_autoware_light</t>
   </si>
   <si>
@@ -71,9 +71,6 @@
     <t>AutowareConfigTemplate_1.xlsx</t>
   </si>
   <si>
-    <t>GoalConfig.xlsx</t>
-  </si>
-  <si>
     <t>SimulinkConfig_1_1.xlsx</t>
   </si>
   <si>
@@ -102,9 +99,6 @@
   </si>
   <si>
     <t>AutowareConfigTemplate_6.xlsx</t>
-  </si>
-  <si>
-    <t>KTH_pedestrian_autoware_light/OpenScenario/Results/Experiment_A1_generated/OpenScenario</t>
   </si>
   <si>
     <t>KTH_pedestrian_autoware_light/OpenScenario/Results/Experiment_A2_generated/OpenScenario</t>
@@ -459,9 +453,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C70A9173-4F80-4F13-9FB2-F870FDE8F443}">
-  <dimension ref="A1:AW8"/>
+  <dimension ref="A1:AW7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A1:XFD8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -474,148 +470,148 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="F1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="G1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="H1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="J1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="K1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="L1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="M1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="N1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="O1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="P1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="Q1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="R1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="S1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="T1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="U1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="V1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="W1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="X1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="Y1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="Z1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AA1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AB1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AC1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AD1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AE1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AF1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AG1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AH1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AI1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AJ1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AK1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AL1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AM1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AN1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AO1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AP1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AQ1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AR1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AS1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AT1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AU1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AV1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AW1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:49" x14ac:dyDescent="0.3">
@@ -933,64 +929,64 @@
         <v>10</v>
       </c>
       <c r="F4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" t="s">
         <v>17</v>
       </c>
-      <c r="G4" t="s">
+      <c r="K4" t="s">
         <v>17</v>
       </c>
-      <c r="H4" t="s">
+      <c r="L4" t="s">
         <v>17</v>
       </c>
-      <c r="I4" t="s">
+      <c r="M4" t="s">
         <v>17</v>
       </c>
-      <c r="J4" t="s">
+      <c r="N4" t="s">
         <v>18</v>
       </c>
-      <c r="K4" t="s">
+      <c r="O4" t="s">
         <v>18</v>
       </c>
-      <c r="L4" t="s">
+      <c r="P4" t="s">
         <v>18</v>
       </c>
-      <c r="M4" t="s">
+      <c r="Q4" t="s">
         <v>18</v>
       </c>
-      <c r="N4" t="s">
+      <c r="R4" t="s">
         <v>19</v>
       </c>
-      <c r="O4" t="s">
+      <c r="S4" t="s">
         <v>19</v>
       </c>
-      <c r="P4" t="s">
+      <c r="T4" t="s">
         <v>19</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="U4" t="s">
         <v>19</v>
       </c>
-      <c r="R4" t="s">
+      <c r="V4" t="s">
         <v>20</v>
       </c>
-      <c r="S4" t="s">
+      <c r="W4" t="s">
         <v>20</v>
       </c>
-      <c r="T4" t="s">
+      <c r="X4" t="s">
         <v>20</v>
       </c>
-      <c r="U4" t="s">
+      <c r="Y4" t="s">
         <v>20</v>
-      </c>
-      <c r="V4" t="s">
-        <v>21</v>
-      </c>
-      <c r="W4" t="s">
-        <v>21</v>
-      </c>
-      <c r="X4" t="s">
-        <v>21</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>21</v>
       </c>
       <c r="Z4" t="s">
         <v>10</v>
@@ -1005,64 +1001,64 @@
         <v>10</v>
       </c>
       <c r="AD4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AH4" t="s">
         <v>17</v>
       </c>
-      <c r="AE4" t="s">
+      <c r="AI4" t="s">
         <v>17</v>
       </c>
-      <c r="AF4" t="s">
+      <c r="AJ4" t="s">
         <v>17</v>
       </c>
-      <c r="AG4" t="s">
+      <c r="AK4" t="s">
         <v>17</v>
       </c>
-      <c r="AH4" t="s">
+      <c r="AL4" t="s">
         <v>18</v>
       </c>
-      <c r="AI4" t="s">
+      <c r="AM4" t="s">
         <v>18</v>
       </c>
-      <c r="AJ4" t="s">
+      <c r="AN4" t="s">
         <v>18</v>
       </c>
-      <c r="AK4" t="s">
+      <c r="AO4" t="s">
         <v>18</v>
       </c>
-      <c r="AL4" t="s">
+      <c r="AP4" t="s">
         <v>19</v>
       </c>
-      <c r="AM4" t="s">
+      <c r="AQ4" t="s">
         <v>19</v>
       </c>
-      <c r="AN4" t="s">
+      <c r="AR4" t="s">
         <v>19</v>
       </c>
-      <c r="AO4" t="s">
+      <c r="AS4" t="s">
         <v>19</v>
       </c>
-      <c r="AP4" t="s">
+      <c r="AT4" t="s">
         <v>20</v>
       </c>
-      <c r="AQ4" t="s">
+      <c r="AU4" t="s">
         <v>20</v>
       </c>
-      <c r="AR4" t="s">
+      <c r="AV4" t="s">
         <v>20</v>
       </c>
-      <c r="AS4" t="s">
+      <c r="AW4" t="s">
         <v>20</v>
-      </c>
-      <c r="AT4" t="s">
-        <v>21</v>
-      </c>
-      <c r="AU4" t="s">
-        <v>21</v>
-      </c>
-      <c r="AV4" t="s">
-        <v>21</v>
-      </c>
-      <c r="AW4" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:49" x14ac:dyDescent="0.3">
@@ -1073,448 +1069,299 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F5" t="s">
         <v>11</v>
       </c>
       <c r="G5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="I5" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="J5" t="s">
         <v>11</v>
       </c>
       <c r="K5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="L5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="M5" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="N5" t="s">
         <v>11</v>
       </c>
       <c r="O5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="P5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="Q5" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="R5" t="s">
         <v>11</v>
       </c>
       <c r="S5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="T5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="U5" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="V5" t="s">
         <v>11</v>
       </c>
       <c r="W5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="X5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="Y5" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="Z5" t="s">
         <v>11</v>
       </c>
       <c r="AA5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="AB5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="AC5" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="AD5" t="s">
         <v>11</v>
       </c>
       <c r="AE5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="AF5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="AG5" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="AH5" t="s">
         <v>11</v>
       </c>
       <c r="AI5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="AJ5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="AK5" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="AL5" t="s">
         <v>11</v>
       </c>
       <c r="AM5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="AN5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="AO5" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="AP5" t="s">
         <v>11</v>
       </c>
       <c r="AQ5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="AR5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="AS5" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="AT5" t="s">
         <v>11</v>
       </c>
       <c r="AU5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="AV5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="AW5" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6" t="s">
-        <v>16</v>
-      </c>
-      <c r="J6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K6" t="s">
-        <v>14</v>
-      </c>
-      <c r="L6" t="s">
-        <v>15</v>
-      </c>
-      <c r="M6" t="s">
-        <v>16</v>
-      </c>
-      <c r="N6" t="s">
-        <v>12</v>
-      </c>
-      <c r="O6" t="s">
-        <v>14</v>
-      </c>
-      <c r="P6" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>16</v>
-      </c>
-      <c r="R6" t="s">
-        <v>12</v>
-      </c>
-      <c r="S6" t="s">
-        <v>14</v>
-      </c>
-      <c r="T6" t="s">
-        <v>15</v>
-      </c>
-      <c r="U6" t="s">
-        <v>16</v>
-      </c>
-      <c r="V6" t="s">
-        <v>12</v>
-      </c>
-      <c r="W6" t="s">
-        <v>14</v>
-      </c>
-      <c r="X6" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>16</v>
-      </c>
-      <c r="Z6" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>14</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AC6" t="s">
-        <v>16</v>
-      </c>
-      <c r="AD6" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE6" t="s">
-        <v>14</v>
-      </c>
-      <c r="AF6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG6" t="s">
-        <v>16</v>
-      </c>
-      <c r="AH6" t="s">
-        <v>12</v>
-      </c>
-      <c r="AI6" t="s">
-        <v>14</v>
-      </c>
-      <c r="AJ6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AK6" t="s">
-        <v>16</v>
-      </c>
-      <c r="AL6" t="s">
-        <v>12</v>
-      </c>
-      <c r="AM6" t="s">
-        <v>14</v>
-      </c>
-      <c r="AN6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AO6" t="s">
-        <v>16</v>
-      </c>
-      <c r="AP6" t="s">
-        <v>12</v>
-      </c>
-      <c r="AQ6" t="s">
-        <v>14</v>
-      </c>
-      <c r="AR6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AS6" t="s">
-        <v>16</v>
-      </c>
-      <c r="AT6" t="s">
-        <v>12</v>
-      </c>
-      <c r="AU6" t="s">
-        <v>14</v>
-      </c>
-      <c r="AV6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AW6" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="7" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:49" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I8" t="s">
-        <v>13</v>
-      </c>
-      <c r="J8" t="s">
-        <v>13</v>
-      </c>
-      <c r="K8" t="s">
-        <v>13</v>
-      </c>
-      <c r="L8" t="s">
-        <v>13</v>
-      </c>
-      <c r="M8" t="s">
-        <v>13</v>
-      </c>
-      <c r="N8" t="s">
-        <v>13</v>
-      </c>
-      <c r="O8" t="s">
-        <v>13</v>
-      </c>
-      <c r="P8" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>13</v>
-      </c>
-      <c r="R8" t="s">
-        <v>13</v>
-      </c>
-      <c r="S8" t="s">
-        <v>13</v>
-      </c>
-      <c r="T8" t="s">
-        <v>13</v>
-      </c>
-      <c r="U8" t="s">
-        <v>13</v>
-      </c>
-      <c r="V8" t="s">
-        <v>13</v>
-      </c>
-      <c r="W8" t="s">
-        <v>13</v>
-      </c>
-      <c r="X8" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AE8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AF8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AG8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AH8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AI8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AJ8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AK8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AL8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AM8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AN8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AO8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AP8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AQ8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AR8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AS8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AT8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AU8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AV8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AW8" t="s">
-        <v>13</v>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" t="s">
+        <v>12</v>
+      </c>
+      <c r="K7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L7" t="s">
+        <v>12</v>
+      </c>
+      <c r="M7" t="s">
+        <v>12</v>
+      </c>
+      <c r="N7" t="s">
+        <v>12</v>
+      </c>
+      <c r="O7" t="s">
+        <v>12</v>
+      </c>
+      <c r="P7" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>12</v>
+      </c>
+      <c r="R7" t="s">
+        <v>12</v>
+      </c>
+      <c r="S7" t="s">
+        <v>12</v>
+      </c>
+      <c r="T7" t="s">
+        <v>12</v>
+      </c>
+      <c r="U7" t="s">
+        <v>12</v>
+      </c>
+      <c r="V7" t="s">
+        <v>12</v>
+      </c>
+      <c r="W7" t="s">
+        <v>12</v>
+      </c>
+      <c r="X7" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG7" t="s">
+        <v>12</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ7" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK7" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL7" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM7" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN7" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO7" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP7" t="s">
+        <v>12</v>
+      </c>
+      <c r="AQ7" t="s">
+        <v>12</v>
+      </c>
+      <c r="AR7" t="s">
+        <v>12</v>
+      </c>
+      <c r="AS7" t="s">
+        <v>12</v>
+      </c>
+      <c r="AT7" t="s">
+        <v>12</v>
+      </c>
+      <c r="AU7" t="s">
+        <v>12</v>
+      </c>
+      <c r="AV7" t="s">
+        <v>12</v>
+      </c>
+      <c r="AW7" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved log in the TA catch
</commit_message>
<xml_diff>
--- a/AD-EYE/TA/Configurations/TAOrder.xlsx
+++ b/AD-EYE/TA/Configurations/TAOrder.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adeye\AD-EYE_Core\AD-EYE\TA\Configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E32F1EBB-46F9-4EBB-860C-28100FB1EBE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64660F40-6A0D-41C9-AD57-F171CCDCCC05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15996" yWindow="1272" windowWidth="14724" windowHeight="12204" xr2:uid="{6A716585-B476-48DA-845D-AAEABE8F85A6}"/>
+    <workbookView xWindow="12396" yWindow="2376" windowWidth="14724" windowHeight="12204" xr2:uid="{6A716585-B476-48DA-845D-AAEABE8F85A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -74,9 +74,6 @@
     <t>SimulinkConfig_1_1.xlsx</t>
   </si>
   <si>
-    <t>ssh</t>
-  </si>
-  <si>
     <t>SimulinkConfig_1_2.xlsx</t>
   </si>
   <si>
@@ -102,6 +99,9 @@
   </si>
   <si>
     <t>KTH_pedestrian_autoware_light/OpenScenario/Results/Experiment_A2_generated/OpenScenario</t>
+  </si>
+  <si>
+    <t>Configurations/SSHConfig.csv</t>
   </si>
 </sst>
 </file>
@@ -455,8 +455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C70A9173-4F80-4F13-9FB2-F870FDE8F443}">
   <dimension ref="A1:AW7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A1:XFD8"/>
+    <sheetView tabSelected="1" topLeftCell="AW1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:AW7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -542,76 +542,76 @@
         <v>7</v>
       </c>
       <c r="Z1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AA1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AB1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AC1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AD1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AE1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AF1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AG1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AH1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AI1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AJ1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AK1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AL1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AM1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AN1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AO1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AP1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AQ1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AR1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AS1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AT1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AU1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AV1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AW1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:49" x14ac:dyDescent="0.3">
@@ -929,64 +929,64 @@
         <v>10</v>
       </c>
       <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" t="s">
         <v>16</v>
       </c>
-      <c r="G4" t="s">
+      <c r="K4" t="s">
         <v>16</v>
       </c>
-      <c r="H4" t="s">
+      <c r="L4" t="s">
         <v>16</v>
       </c>
-      <c r="I4" t="s">
+      <c r="M4" t="s">
         <v>16</v>
       </c>
-      <c r="J4" t="s">
+      <c r="N4" t="s">
         <v>17</v>
       </c>
-      <c r="K4" t="s">
+      <c r="O4" t="s">
         <v>17</v>
       </c>
-      <c r="L4" t="s">
+      <c r="P4" t="s">
         <v>17</v>
       </c>
-      <c r="M4" t="s">
+      <c r="Q4" t="s">
         <v>17</v>
       </c>
-      <c r="N4" t="s">
+      <c r="R4" t="s">
         <v>18</v>
       </c>
-      <c r="O4" t="s">
+      <c r="S4" t="s">
         <v>18</v>
       </c>
-      <c r="P4" t="s">
+      <c r="T4" t="s">
         <v>18</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="U4" t="s">
         <v>18</v>
       </c>
-      <c r="R4" t="s">
+      <c r="V4" t="s">
         <v>19</v>
       </c>
-      <c r="S4" t="s">
+      <c r="W4" t="s">
         <v>19</v>
       </c>
-      <c r="T4" t="s">
+      <c r="X4" t="s">
         <v>19</v>
       </c>
-      <c r="U4" t="s">
+      <c r="Y4" t="s">
         <v>19</v>
-      </c>
-      <c r="V4" t="s">
-        <v>20</v>
-      </c>
-      <c r="W4" t="s">
-        <v>20</v>
-      </c>
-      <c r="X4" t="s">
-        <v>20</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>20</v>
       </c>
       <c r="Z4" t="s">
         <v>10</v>
@@ -1001,64 +1001,64 @@
         <v>10</v>
       </c>
       <c r="AD4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH4" t="s">
         <v>16</v>
       </c>
-      <c r="AE4" t="s">
+      <c r="AI4" t="s">
         <v>16</v>
       </c>
-      <c r="AF4" t="s">
+      <c r="AJ4" t="s">
         <v>16</v>
       </c>
-      <c r="AG4" t="s">
+      <c r="AK4" t="s">
         <v>16</v>
       </c>
-      <c r="AH4" t="s">
+      <c r="AL4" t="s">
         <v>17</v>
       </c>
-      <c r="AI4" t="s">
+      <c r="AM4" t="s">
         <v>17</v>
       </c>
-      <c r="AJ4" t="s">
+      <c r="AN4" t="s">
         <v>17</v>
       </c>
-      <c r="AK4" t="s">
+      <c r="AO4" t="s">
         <v>17</v>
       </c>
-      <c r="AL4" t="s">
+      <c r="AP4" t="s">
         <v>18</v>
       </c>
-      <c r="AM4" t="s">
+      <c r="AQ4" t="s">
         <v>18</v>
       </c>
-      <c r="AN4" t="s">
+      <c r="AR4" t="s">
         <v>18</v>
       </c>
-      <c r="AO4" t="s">
+      <c r="AS4" t="s">
         <v>18</v>
       </c>
-      <c r="AP4" t="s">
+      <c r="AT4" t="s">
         <v>19</v>
       </c>
-      <c r="AQ4" t="s">
+      <c r="AU4" t="s">
         <v>19</v>
       </c>
-      <c r="AR4" t="s">
+      <c r="AV4" t="s">
         <v>19</v>
       </c>
-      <c r="AS4" t="s">
+      <c r="AW4" t="s">
         <v>19</v>
-      </c>
-      <c r="AT4" t="s">
-        <v>20</v>
-      </c>
-      <c r="AU4" t="s">
-        <v>20</v>
-      </c>
-      <c r="AV4" t="s">
-        <v>20</v>
-      </c>
-      <c r="AW4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:49" x14ac:dyDescent="0.3">
@@ -1069,145 +1069,145 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>14</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
       </c>
       <c r="F5" t="s">
         <v>11</v>
       </c>
       <c r="G5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" t="s">
         <v>13</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>14</v>
-      </c>
-      <c r="I5" t="s">
-        <v>15</v>
       </c>
       <c r="J5" t="s">
         <v>11</v>
       </c>
       <c r="K5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L5" t="s">
         <v>13</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>14</v>
-      </c>
-      <c r="M5" t="s">
-        <v>15</v>
       </c>
       <c r="N5" t="s">
         <v>11</v>
       </c>
       <c r="O5" t="s">
+        <v>12</v>
+      </c>
+      <c r="P5" t="s">
         <v>13</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>14</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>15</v>
       </c>
       <c r="R5" t="s">
         <v>11</v>
       </c>
       <c r="S5" t="s">
+        <v>12</v>
+      </c>
+      <c r="T5" t="s">
         <v>13</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>14</v>
-      </c>
-      <c r="U5" t="s">
-        <v>15</v>
       </c>
       <c r="V5" t="s">
         <v>11</v>
       </c>
       <c r="W5" t="s">
+        <v>12</v>
+      </c>
+      <c r="X5" t="s">
         <v>13</v>
       </c>
-      <c r="X5" t="s">
+      <c r="Y5" t="s">
         <v>14</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>15</v>
       </c>
       <c r="Z5" t="s">
         <v>11</v>
       </c>
       <c r="AA5" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB5" t="s">
         <v>13</v>
       </c>
-      <c r="AB5" t="s">
+      <c r="AC5" t="s">
         <v>14</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>15</v>
       </c>
       <c r="AD5" t="s">
         <v>11</v>
       </c>
       <c r="AE5" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF5" t="s">
         <v>13</v>
       </c>
-      <c r="AF5" t="s">
+      <c r="AG5" t="s">
         <v>14</v>
-      </c>
-      <c r="AG5" t="s">
-        <v>15</v>
       </c>
       <c r="AH5" t="s">
         <v>11</v>
       </c>
       <c r="AI5" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ5" t="s">
         <v>13</v>
       </c>
-      <c r="AJ5" t="s">
+      <c r="AK5" t="s">
         <v>14</v>
-      </c>
-      <c r="AK5" t="s">
-        <v>15</v>
       </c>
       <c r="AL5" t="s">
         <v>11</v>
       </c>
       <c r="AM5" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN5" t="s">
         <v>13</v>
       </c>
-      <c r="AN5" t="s">
+      <c r="AO5" t="s">
         <v>14</v>
-      </c>
-      <c r="AO5" t="s">
-        <v>15</v>
       </c>
       <c r="AP5" t="s">
         <v>11</v>
       </c>
       <c r="AQ5" t="s">
+        <v>12</v>
+      </c>
+      <c r="AR5" t="s">
         <v>13</v>
       </c>
-      <c r="AR5" t="s">
+      <c r="AS5" t="s">
         <v>14</v>
-      </c>
-      <c r="AS5" t="s">
-        <v>15</v>
       </c>
       <c r="AT5" t="s">
         <v>11</v>
       </c>
       <c r="AU5" t="s">
+        <v>12</v>
+      </c>
+      <c r="AV5" t="s">
         <v>13</v>
       </c>
-      <c r="AV5" t="s">
+      <c r="AW5" t="s">
         <v>14</v>
-      </c>
-      <c r="AW5" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:49" x14ac:dyDescent="0.3">
@@ -1220,148 +1220,148 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="F7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="G7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="H7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="I7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="J7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="K7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="L7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="M7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="N7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="O7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="P7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="Q7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="R7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="S7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="T7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="U7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="V7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="W7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="X7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="Y7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="Z7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="AA7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="AB7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="AC7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="AD7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="AE7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="AF7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="AG7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="AH7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="AI7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="AJ7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="AK7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="AL7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="AM7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="AN7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="AO7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="AP7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="AQ7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="AR7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="AS7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="AT7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="AU7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="AV7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="AW7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>